<commit_message>
metadata entry and updating matrix
</commit_message>
<xml_diff>
--- a/data vis /variability metadata.xlsx
+++ b/data vis /variability metadata.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/summer2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/summer2020/data vis /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD72F53-2872-5248-955C-D5CC4AB35446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA77A48-F05F-2846-A258-4415CC520E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="27640" windowHeight="15460" xr2:uid="{6BFC6FC5-5213-6546-AFED-C42FCE96236D}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15460" xr2:uid="{6BFC6FC5-5213-6546-AFED-C42FCE96236D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t>study id</t>
   </si>
@@ -94,16 +94,240 @@
   </si>
   <si>
     <t>mean of 25 or 18 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data availability </t>
+  </si>
+  <si>
+    <t>khelifa_2019</t>
+  </si>
+  <si>
+    <t>descamps-julien_2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long_2007 </t>
+  </si>
+  <si>
+    <t>orland_2004</t>
+  </si>
+  <si>
+    <t>gonzalez&amp;holt_2002</t>
+  </si>
+  <si>
+    <t>matthews_2007</t>
+  </si>
+  <si>
+    <t>fontaine&amp;gonzalez_2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pushkar_2010 </t>
+  </si>
+  <si>
+    <t>seuffert_2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">du_2003 </t>
+  </si>
+  <si>
+    <t>petavy_2001</t>
+  </si>
+  <si>
+    <t>hilbeck_1998</t>
+  </si>
+  <si>
+    <t>shrode_1977</t>
+  </si>
+  <si>
+    <t>resilva_2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peng_2014 </t>
+  </si>
+  <si>
+    <t>zhao_2014</t>
+  </si>
+  <si>
+    <t>foray_2014</t>
+  </si>
+  <si>
+    <t>klepsatel_2013</t>
+  </si>
+  <si>
+    <t>duncan_2011</t>
+  </si>
+  <si>
+    <t>radmacher_2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barfield_1978 </t>
+  </si>
+  <si>
+    <t>butler_1980</t>
+  </si>
+  <si>
+    <t>butler_1966</t>
+  </si>
+  <si>
+    <t>butler_1968</t>
+  </si>
+  <si>
+    <t>davis_2006</t>
+  </si>
+  <si>
+    <t>eubank_1973</t>
+  </si>
+  <si>
+    <t>fielding_1988</t>
+  </si>
+  <si>
+    <t>hagstrum_1991</t>
+  </si>
+  <si>
+    <t>harries_1948</t>
+  </si>
+  <si>
+    <t>joshi_1996</t>
+  </si>
+  <si>
+    <t>kingsolver_2015</t>
+  </si>
+  <si>
+    <t>lin_1954</t>
+  </si>
+  <si>
+    <t>ludwig_1933</t>
+  </si>
+  <si>
+    <t>messenger_1969</t>
+  </si>
+  <si>
+    <t>niehaus_2012</t>
+  </si>
+  <si>
+    <t>siddiqui_1972</t>
+  </si>
+  <si>
+    <t>simonet_1981</t>
+  </si>
+  <si>
+    <t>petchey_2000</t>
+  </si>
+  <si>
+    <t>petchey_2002</t>
+  </si>
+  <si>
+    <t>gonzalez_2004</t>
+  </si>
+  <si>
+    <t>luckinbill_1978</t>
+  </si>
+  <si>
+    <t>laakso_2003</t>
+  </si>
+  <si>
+    <t>estay_2011</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>data availability links</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5061/dryad.fc75292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y </t>
+  </si>
+  <si>
+    <t>https://figshare.com/collections/STABLE_COEXISTENCE_IN_A_FLUCTUATING_ENVIRONMENT_AN_EXPERIMENTAL_DEMONSTRATION/3298823</t>
+  </si>
+  <si>
+    <t>data location</t>
+  </si>
+  <si>
+    <t>dryad</t>
+  </si>
+  <si>
+    <t>figshare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+  </si>
+  <si>
+    <t xml:space="preserve">indvidual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">development rate </t>
+  </si>
+  <si>
+    <t>temp amplitude</t>
+  </si>
+  <si>
+    <t>18, plus or minus 3 or 7 degrees</t>
+  </si>
+  <si>
+    <t>TPC, applicability of TPC from constant or flux environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negligible differences between temperature controlled constant and fluctuating treatments when accounting for non-linearities, the stochastic natural treatment did not line up with TPC in lab </t>
+  </si>
+  <si>
+    <t>TPC</t>
+  </si>
+  <si>
+    <t>coexistence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population, community </t>
+  </si>
+  <si>
+    <t>population density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp color </t>
+  </si>
+  <si>
+    <t xml:space="preserve">white or red </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color of environmental noise, coexistence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp variation encourages persistance of two species on one limiting resource?, though coexistence is not strongly sensitive to periodicity of flux </t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">community </t>
+  </si>
+  <si>
+    <t>immigration, competition</t>
+  </si>
+  <si>
+    <t>competition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,13 +350,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,15 +672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F1B9DB-E956-9840-8A22-A19B07644F01}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,51 +717,198 @@
       <c r="L1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -568,8 +942,311 @@
       <c r="L10" t="s">
         <v>20</v>
       </c>
+      <c r="M10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{50CE8097-31AD-974B-B0CE-9E409BB4A1EA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to file classification, standardizing organization level based on response variable
</commit_message>
<xml_diff>
--- a/data vis /variability metadata.xlsx
+++ b/data vis /variability metadata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/summer2020/data vis /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA77A48-F05F-2846-A258-4415CC520E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0168E4FF-53C8-C742-A6BA-D07F0AF07757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15460" xr2:uid="{6BFC6FC5-5213-6546-AFED-C42FCE96236D}"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="27640" windowHeight="15460" xr2:uid="{6BFC6FC5-5213-6546-AFED-C42FCE96236D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="101">
   <si>
     <t>study id</t>
   </si>
@@ -310,6 +311,24 @@
   </si>
   <si>
     <t>competition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population </t>
+  </si>
+  <si>
+    <t xml:space="preserve">population density, population variability </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nutrient level </t>
+  </si>
+  <si>
+    <t>about of prey available</t>
+  </si>
+  <si>
+    <t>fluctuation color</t>
+  </si>
+  <si>
+    <t>temporally autcorrelated variability enhanced the effect of immgration, "inflationary effect"</t>
   </si>
 </sst>
 </file>
@@ -675,7 +694,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,6 +868,9 @@
       <c r="K4" t="s">
         <v>94</v>
       </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
       <c r="M4" t="s">
         <v>75</v>
       </c>
@@ -859,6 +881,21 @@
       </c>
       <c r="B5" t="s">
         <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
       </c>
       <c r="M5" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
commiting to avoid merge conflicts
</commit_message>
<xml_diff>
--- a/data vis /variability metadata.xlsx
+++ b/data vis /variability metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/summer2020/data vis /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A3C64-A9B7-044A-BA28-33DAD4371B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{399723BB-4085-504E-ABD1-1B687EFCE424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36040" yWindow="-12700" windowWidth="27640" windowHeight="16600" xr2:uid="{6BFC6FC5-5213-6546-AFED-C42FCE96236D}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="column info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1158,8 +1159,8 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A46"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>